<commit_message>
T-079: implement supplier list simplified single-sheet template
</commit_message>
<xml_diff>
--- a/templates/excel/omts-supplier-list-example.xlsx
+++ b/templates/excel/omts-supplier-list-example.xlsx
@@ -701,11 +701,6 @@
           <t>EUR</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>7317ABCDE1234567890</t>
-        </is>
-      </c>
       <c r="O6" t="inlineStr">
         <is>
           <t>medium</t>

</xml_diff>